<commit_message>
Added TestCase in Card Unit Testing
</commit_message>
<xml_diff>
--- a/GroupProjects/Simple_ATM/Card_ECU/Unit Tests/App/Card/TestCases.xlsx
+++ b/GroupProjects/Simple_ATM/Card_ECU/Unit Tests/App/Card/TestCases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Mohamed Sprints\sprints-2021\GroupProjects\Simple_ATM\Card_ECU\Unit Tests\App\Card\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CED8436-49EA-49B1-BC65-41D045B81D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A53AF9D-8CC0-4FDC-84AB-583FDBA67C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56237F82-C67E-4D5F-9511-A6B1695E74E7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Test ID</t>
   </si>
@@ -89,6 +89,15 @@
   </si>
   <si>
     <t>Set Card Data In Memory On Receiving ADMIN from Terminal</t>
+  </si>
+  <si>
+    <t>CARD_006</t>
+  </si>
+  <si>
+    <t>Doesn't Change Card Data In Memory if didn’t receive ADMIN from Terminal</t>
+  </si>
+  <si>
+    <t>Card Data  Isn't Changed in memory</t>
   </si>
 </sst>
 </file>
@@ -162,8 +171,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{695F2E12-D1DC-44C3-8F40-FD7F8B86FA9F}" name="Table1" displayName="Table1" ref="A1:E6" totalsRowShown="0" tableBorderDxfId="1" headerRowCellStyle="Normal">
-  <autoFilter ref="A1:E6" xr:uid="{695F2E12-D1DC-44C3-8F40-FD7F8B86FA9F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{695F2E12-D1DC-44C3-8F40-FD7F8B86FA9F}" name="Table1" displayName="Table1" ref="A1:E7" totalsRowShown="0" tableBorderDxfId="1" headerRowCellStyle="Normal">
+  <autoFilter ref="A1:E7" xr:uid="{695F2E12-D1DC-44C3-8F40-FD7F8B86FA9F}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B8DEECCF-9FB7-47FD-B55B-0A768F33B550}" name="Test ID"/>
     <tableColumn id="2" xr3:uid="{20E110E4-5360-4262-BEC4-A07BEF421B26}" name="Test Summary"/>
@@ -475,13 +484,13 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="52.8984375" customWidth="1"/>
+    <col min="2" max="2" width="63.59765625" customWidth="1"/>
     <col min="3" max="3" width="45.5" customWidth="1"/>
     <col min="4" max="4" width="21.19921875" customWidth="1"/>
     <col min="5" max="5" width="22.59765625" customWidth="1"/>
@@ -519,7 +528,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="1">
-        <v>44413</v>
+        <v>44414</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -537,7 +546,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="1">
-        <v>44413</v>
+        <v>44414</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -555,7 +564,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="1">
-        <v>44413</v>
+        <v>44414</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -573,7 +582,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="1">
-        <v>44413</v>
+        <v>44414</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -591,11 +600,26 @@
         <v>4</v>
       </c>
       <c r="E6" s="1">
-        <v>44413</v>
+        <v>44414</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44414</v>
+      </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
All Unit Tests Added
</commit_message>
<xml_diff>
--- a/GroupProjects/Simple_ATM/Card_ECU/Unit Tests/App/Card/TestCases.xlsx
+++ b/GroupProjects/Simple_ATM/Card_ECU/Unit Tests/App/Card/TestCases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Mohamed Sprints\sprints-2021\GroupProjects\Simple_ATM\Card_ECU\Unit Tests\App\Card\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A53AF9D-8CC0-4FDC-84AB-583FDBA67C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CED8436-49EA-49B1-BC65-41D045B81D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56237F82-C67E-4D5F-9511-A6B1695E74E7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Test ID</t>
   </si>
@@ -89,15 +89,6 @@
   </si>
   <si>
     <t>Set Card Data In Memory On Receiving ADMIN from Terminal</t>
-  </si>
-  <si>
-    <t>CARD_006</t>
-  </si>
-  <si>
-    <t>Doesn't Change Card Data In Memory if didn’t receive ADMIN from Terminal</t>
-  </si>
-  <si>
-    <t>Card Data  Isn't Changed in memory</t>
   </si>
 </sst>
 </file>
@@ -171,8 +162,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{695F2E12-D1DC-44C3-8F40-FD7F8B86FA9F}" name="Table1" displayName="Table1" ref="A1:E7" totalsRowShown="0" tableBorderDxfId="1" headerRowCellStyle="Normal">
-  <autoFilter ref="A1:E7" xr:uid="{695F2E12-D1DC-44C3-8F40-FD7F8B86FA9F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{695F2E12-D1DC-44C3-8F40-FD7F8B86FA9F}" name="Table1" displayName="Table1" ref="A1:E6" totalsRowShown="0" tableBorderDxfId="1" headerRowCellStyle="Normal">
+  <autoFilter ref="A1:E6" xr:uid="{695F2E12-D1DC-44C3-8F40-FD7F8B86FA9F}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B8DEECCF-9FB7-47FD-B55B-0A768F33B550}" name="Test ID"/>
     <tableColumn id="2" xr3:uid="{20E110E4-5360-4262-BEC4-A07BEF421B26}" name="Test Summary"/>
@@ -484,13 +475,13 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="63.59765625" customWidth="1"/>
+    <col min="2" max="2" width="52.8984375" customWidth="1"/>
     <col min="3" max="3" width="45.5" customWidth="1"/>
     <col min="4" max="4" width="21.19921875" customWidth="1"/>
     <col min="5" max="5" width="22.59765625" customWidth="1"/>
@@ -528,7 +519,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="1">
-        <v>44414</v>
+        <v>44413</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -546,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="1">
-        <v>44414</v>
+        <v>44413</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -564,7 +555,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="1">
-        <v>44414</v>
+        <v>44413</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -582,7 +573,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="1">
-        <v>44414</v>
+        <v>44413</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -600,26 +591,11 @@
         <v>4</v>
       </c>
       <c r="E6" s="1">
-        <v>44414</v>
+        <v>44413</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1">
-        <v>44414</v>
-      </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>